<commit_message>
close #174: Fix verify_ids_sp_description_values ​​non-string values ​​check
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/valores.xlsx
+++ b/input_data/data_ground_truth_01/valores.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="valores" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="valores" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -300,44 +300,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -413,8 +417,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -423,1134 +533,1134 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="24.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="3" style="3" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="4" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="10" t="n">
         <v>0.679501771703989</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="10" t="n">
         <v>0.679501771703989</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="10" t="n">
         <v>0.635045214513727</v>
       </c>
-      <c r="F2" s="9" t="n">
+      <c r="F2" s="10" t="n">
         <v>0.703511665266981</v>
       </c>
-      <c r="G2" s="9" t="n">
+      <c r="G2" s="10" t="n">
         <v>0.689404949258627</v>
       </c>
-      <c r="H2" s="9" t="n">
+      <c r="H2" s="10" t="n">
         <v>0.806633367915323</v>
       </c>
-      <c r="I2" s="9" t="n">
+      <c r="I2" s="10" t="n">
         <v>0.251806216454027</v>
       </c>
-      <c r="J2" s="9" t="n">
+      <c r="J2" s="10" t="n">
         <v>0.3</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="K2" s="10" t="n">
         <v>0.46</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="M2" s="9" t="n">
+      <c r="M2" s="10" t="n">
         <v>0.51</v>
       </c>
-      <c r="N2" s="9" t="n">
+      <c r="N2" s="10" t="n">
         <v>0.48</v>
       </c>
-      <c r="O2" s="9" t="n">
+      <c r="O2" s="10" t="n">
         <v>0.690607281794881</v>
       </c>
-      <c r="P2" s="9" t="n">
+      <c r="P2" s="10" t="n">
         <v>0.187168284406015</v>
       </c>
-      <c r="Q2" s="9" t="n">
+      <c r="Q2" s="10" t="n">
         <v>0.172675984067355</v>
       </c>
-      <c r="R2" s="9" t="n">
+      <c r="R2" s="10" t="n">
         <v>0.643464893806262</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="10" t="n">
         <v>0.646593807126705</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="10" t="n">
         <v>0.646593807126705</v>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="10" t="n">
         <v>0.62493263841433</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="10" t="n">
         <v>0.62493263841433</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="10" t="n">
         <v>0.671110098170615</v>
       </c>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="10" t="n">
         <v>0.530039492274218</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="10" t="n">
         <v>0.340063415171096</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="10" t="n">
         <v>0.26</v>
       </c>
-      <c r="K3" s="9" t="n">
+      <c r="K3" s="10" t="n">
         <v>0.45</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="M3" s="9" t="n">
+      <c r="M3" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="N3" s="9" t="n">
+      <c r="N3" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="O3" s="9" t="n">
+      <c r="O3" s="10" t="n">
         <v>0.570991130092722</v>
       </c>
-      <c r="P3" s="9" t="n">
+      <c r="P3" s="10" t="n">
         <v>0.592939614220435</v>
       </c>
-      <c r="Q3" s="9" t="n">
+      <c r="Q3" s="10" t="n">
         <v>0.169848598505876</v>
       </c>
-      <c r="R3" s="9" t="n">
+      <c r="R3" s="10" t="n">
         <v>0.536406518021754</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <v>0.74796276549555</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="10" t="n">
         <v>0.74796276549555</v>
       </c>
-      <c r="E4" s="9" t="n">
+      <c r="E4" s="10" t="n">
         <v>0.720555883855326</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="10" t="n">
         <v>0.714664694492201</v>
       </c>
-      <c r="G4" s="9" t="n">
+      <c r="G4" s="10" t="n">
         <v>0.742733566765675</v>
       </c>
-      <c r="H4" s="9" t="n">
+      <c r="H4" s="10" t="n">
         <v>0.707553404923502</v>
       </c>
-      <c r="I4" s="9" t="n">
+      <c r="I4" s="10" t="n">
         <v>0.393826665385519</v>
       </c>
-      <c r="J4" s="9" t="n">
+      <c r="J4" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="10" t="n">
         <v>0.45</v>
       </c>
-      <c r="L4" s="9" t="n">
+      <c r="L4" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="M4" s="9" t="n">
+      <c r="M4" s="10" t="n">
         <v>0.39</v>
       </c>
-      <c r="N4" s="9" t="n">
+      <c r="N4" s="10" t="n">
         <v>0.44</v>
       </c>
-      <c r="O4" s="9" t="n">
+      <c r="O4" s="10" t="n">
         <v>0.690607281794881</v>
       </c>
-      <c r="P4" s="9" t="n">
+      <c r="P4" s="10" t="n">
         <v>0.408596234199239</v>
       </c>
-      <c r="Q4" s="9" t="n">
+      <c r="Q4" s="10" t="n">
         <v>0.244685832976119</v>
       </c>
-      <c r="R4" s="9" t="n">
+      <c r="R4" s="10" t="n">
         <v>0.688585905681939</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <v>0.729582203886894</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="10" t="n">
         <v>0.729582203886894</v>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="10" t="n">
         <v>0.702629350782218</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="10" t="n">
         <v>0.71841096024771</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <v>0.706676227578738</v>
       </c>
-      <c r="H5" s="9" t="n">
+      <c r="H5" s="10" t="n">
         <v>0.471292830322615</v>
       </c>
-      <c r="I5" s="9" t="n">
+      <c r="I5" s="10" t="n">
         <v>0.384149574445352</v>
       </c>
-      <c r="J5" s="9" t="n">
+      <c r="J5" s="10" t="n">
         <v>0.26</v>
       </c>
-      <c r="K5" s="9" t="n">
+      <c r="K5" s="10" t="n">
         <v>0.64</v>
       </c>
-      <c r="L5" s="9" t="n">
+      <c r="L5" s="10" t="n">
         <v>0.57</v>
       </c>
-      <c r="M5" s="9" t="n">
+      <c r="M5" s="10" t="n">
         <v>0.61</v>
       </c>
-      <c r="N5" s="9" t="n">
+      <c r="N5" s="10" t="n">
         <v>0.58</v>
       </c>
-      <c r="O5" s="9" t="n">
+      <c r="O5" s="10" t="n">
         <v>0.437104537763042</v>
       </c>
-      <c r="P5" s="9" t="n">
+      <c r="P5" s="10" t="n">
         <v>0.486520699002306</v>
       </c>
-      <c r="Q5" s="9" t="n">
+      <c r="Q5" s="10" t="n">
         <v>0.505871329785902</v>
       </c>
-      <c r="R5" s="9" t="n">
+      <c r="R5" s="10" t="n">
         <v>0.28745357215629</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <v>0.709424839994261</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="10" t="n">
         <v>0.709424839994261</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="10" t="n">
         <v>0.69834229067696</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="10" t="n">
         <v>0.720003459389335</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="10" t="n">
         <v>0.779055534730612</v>
       </c>
-      <c r="H6" s="9" t="n">
+      <c r="H6" s="10" t="n">
         <v>0.613497325278628</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="10" t="n">
         <v>0.402780183949449</v>
       </c>
-      <c r="J6" s="9" t="n">
+      <c r="J6" s="10" t="n">
         <v>0.26</v>
       </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="10" t="n">
         <v>0.43</v>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="M6" s="9" t="n">
+      <c r="M6" s="10" t="n">
         <v>0.45</v>
       </c>
-      <c r="N6" s="9" t="n">
+      <c r="N6" s="10" t="n">
         <v>0.58</v>
       </c>
-      <c r="O6" s="9" t="n">
+      <c r="O6" s="10" t="n">
         <v>0.437104537763042</v>
       </c>
-      <c r="P6" s="9" t="n">
+      <c r="P6" s="10" t="n">
         <v>0.168716283067166</v>
       </c>
-      <c r="Q6" s="9" t="n">
+      <c r="Q6" s="10" t="n">
         <v>0.275329151445951</v>
       </c>
-      <c r="R6" s="9" t="n">
+      <c r="R6" s="10" t="n">
         <v>0.455040552474789</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <v>0.603290170379874</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="10" t="n">
         <v>0.603290170379874</v>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E7" s="10" t="n">
         <v>0.573796372951498</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="10" t="n">
         <v>0.554120752327722</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G7" s="10" t="n">
         <v>0.540014036319368</v>
       </c>
-      <c r="H7" s="9" t="n">
+      <c r="H7" s="10" t="n">
         <v>0.6245220950403</v>
       </c>
-      <c r="I7" s="9" t="n">
+      <c r="I7" s="10" t="n">
         <v>0.256720852226934</v>
       </c>
-      <c r="J7" s="9" t="n">
+      <c r="J7" s="10" t="n">
         <v>0.36</v>
       </c>
-      <c r="K7" s="9" t="n">
+      <c r="K7" s="10" t="n">
         <v>0.42</v>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="10" t="n">
         <v>0.37</v>
       </c>
-      <c r="M7" s="9" t="n">
+      <c r="M7" s="10" t="n">
         <v>0.34</v>
       </c>
-      <c r="N7" s="9" t="n">
+      <c r="N7" s="10" t="n">
         <v>0.32</v>
       </c>
-      <c r="O7" s="9" t="n">
+      <c r="O7" s="10" t="n">
         <v>0.448795304117594</v>
       </c>
-      <c r="P7" s="9" t="n">
+      <c r="P7" s="10" t="n">
         <v>0.164833996329523</v>
       </c>
-      <c r="Q7" s="9" t="n">
+      <c r="Q7" s="10" t="n">
         <v>0.447817294476809</v>
       </c>
-      <c r="R7" s="9" t="n">
+      <c r="R7" s="10" t="n">
         <v>0.520483055185772</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="10" t="n">
         <v>0.659605568654101</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="10" t="n">
         <v>0.659605568654101</v>
       </c>
-      <c r="E8" s="9" t="n">
+      <c r="E8" s="10" t="n">
         <v>0.617181247531227</v>
       </c>
-      <c r="F8" s="9" t="n">
+      <c r="F8" s="10" t="n">
         <v>0.605245833909201</v>
       </c>
-      <c r="G8" s="9" t="n">
+      <c r="G8" s="10" t="n">
         <v>0.644588129171452</v>
       </c>
-      <c r="H8" s="9" t="n">
+      <c r="H8" s="10" t="n">
         <v>0.674764694253153</v>
       </c>
-      <c r="I8" s="9" t="n">
+      <c r="I8" s="10" t="n">
         <v>0.264833164380987</v>
       </c>
-      <c r="J8" s="9" t="n">
+      <c r="J8" s="10" t="n">
         <v>0.34</v>
       </c>
-      <c r="K8" s="9" t="n">
+      <c r="K8" s="10" t="n">
         <v>0.48</v>
       </c>
-      <c r="L8" s="9" t="n">
+      <c r="L8" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="M8" s="9" t="n">
+      <c r="M8" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="N8" s="9" t="n">
+      <c r="N8" s="10" t="n">
         <v>0.45</v>
       </c>
-      <c r="O8" s="9" t="n">
+      <c r="O8" s="10" t="n">
         <v>0.611733514608378</v>
       </c>
-      <c r="P8" s="9" t="n">
+      <c r="P8" s="10" t="n">
         <v>0.341837704892334</v>
       </c>
-      <c r="Q8" s="9" t="n">
+      <c r="Q8" s="10" t="n">
         <v>0.197632001228399</v>
       </c>
-      <c r="R8" s="9" t="n">
+      <c r="R8" s="10" t="n">
         <v>0.565943829798232</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="10" t="n">
         <v>0.450574993784121</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="10" t="n">
         <v>0.450574993784121</v>
       </c>
-      <c r="E9" s="9" t="n">
+      <c r="E9" s="10" t="n">
         <v>0.425394823400742</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="10" t="n">
         <v>0.473294445392395</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="10" t="n">
         <v>0.431949892103335</v>
       </c>
-      <c r="H9" s="9" t="n">
+      <c r="H9" s="10" t="n">
         <v>0.56910855849017</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="10" t="n">
         <v>0.157387102371809</v>
       </c>
-      <c r="J9" s="9" t="n">
+      <c r="J9" s="10" t="n">
         <v>0.24</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K9" s="10" t="n">
         <v>0.39</v>
       </c>
-      <c r="L9" s="9" t="n">
+      <c r="L9" s="10" t="n">
         <v>0.35</v>
       </c>
-      <c r="M9" s="9" t="n">
+      <c r="M9" s="10" t="n">
         <v>0.43</v>
       </c>
-      <c r="N9" s="9" t="n">
+      <c r="N9" s="10" t="n">
         <v>0.36</v>
       </c>
-      <c r="O9" s="9" t="n">
+      <c r="O9" s="10" t="n">
         <v>0.513344930517577</v>
       </c>
-      <c r="P9" s="9" t="n">
+      <c r="P9" s="10" t="n">
         <v>0.403278779601266</v>
       </c>
-      <c r="Q9" s="9" t="n">
+      <c r="Q9" s="10" t="n">
         <v>0.494614320784849</v>
       </c>
-      <c r="R9" s="9" t="n">
+      <c r="R9" s="10" t="n">
         <v>0.165551792937168</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="10" t="n">
         <v>0.470275035697477</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="10" t="n">
         <v>0.470275035697477</v>
       </c>
-      <c r="E10" s="9" t="n">
+      <c r="E10" s="10" t="n">
         <v>0.426858433537221</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="10" t="n">
         <v>0.438495335828194</v>
       </c>
-      <c r="G10" s="9" t="n">
+      <c r="G10" s="10" t="n">
         <v>0.475173944023219</v>
       </c>
-      <c r="H10" s="9" t="n">
+      <c r="H10" s="10" t="n">
         <v>0.512569859338716</v>
       </c>
-      <c r="I10" s="9" t="n">
+      <c r="I10" s="10" t="n">
         <v>0.157814290806917</v>
       </c>
-      <c r="J10" s="9" t="n">
+      <c r="J10" s="10" t="n">
         <v>0.29</v>
       </c>
-      <c r="K10" s="9" t="n">
+      <c r="K10" s="10" t="n">
         <v>0.47</v>
       </c>
-      <c r="L10" s="9" t="n">
+      <c r="L10" s="10" t="n">
         <v>0.39</v>
       </c>
-      <c r="M10" s="9" t="n">
+      <c r="M10" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="N10" s="9" t="n">
+      <c r="N10" s="10" t="n">
         <v>0.48</v>
       </c>
-      <c r="O10" s="9" t="n">
+      <c r="O10" s="10" t="n">
         <v>0.437104537763042</v>
       </c>
-      <c r="P10" s="9" t="n">
+      <c r="P10" s="10" t="n">
         <v>0.394273107939467</v>
       </c>
-      <c r="Q10" s="9" t="n">
+      <c r="Q10" s="10" t="n">
         <v>0.172885709577704</v>
       </c>
-      <c r="R10" s="9" t="n">
+      <c r="R10" s="10" t="n">
         <v>0.46136777988458</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="10" t="n">
         <v>0.646413908506119</v>
       </c>
-      <c r="D11" s="9" t="n">
+      <c r="D11" s="10" t="n">
         <v>0.646413908506119</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="10" t="n">
         <v>0.631066178619336</v>
       </c>
-      <c r="F11" s="9" t="n">
+      <c r="F11" s="10" t="n">
         <v>0.59695308208696</v>
       </c>
-      <c r="G11" s="9" t="n">
+      <c r="G11" s="10" t="n">
         <v>0.636295377349211</v>
       </c>
-      <c r="H11" s="9" t="n">
+      <c r="H11" s="10" t="n">
         <v>0.499831832496426</v>
       </c>
-      <c r="I11" s="9" t="n">
+      <c r="I11" s="10" t="n">
         <v>0.345198133949</v>
       </c>
-      <c r="J11" s="9" t="n">
+      <c r="J11" s="10" t="n">
         <v>0.33</v>
       </c>
-      <c r="K11" s="9" t="n">
+      <c r="K11" s="10" t="n">
         <v>0.47</v>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="10" t="n">
         <v>0.44</v>
       </c>
-      <c r="M11" s="9" t="n">
+      <c r="M11" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="N11" s="9" t="n">
+      <c r="N11" s="10" t="n">
         <v>0.45</v>
       </c>
-      <c r="O11" s="9" t="n">
+      <c r="O11" s="10" t="n">
         <v>0.437104537763042</v>
       </c>
-      <c r="P11" s="9" t="n">
+      <c r="P11" s="10" t="n">
         <v>0.422740570814199</v>
       </c>
-      <c r="Q11" s="9" t="n">
+      <c r="Q11" s="10" t="n">
         <v>0.147701611286079</v>
       </c>
-      <c r="R11" s="9" t="n">
+      <c r="R11" s="10" t="n">
         <v>0.628052529778176</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="10" t="n">
         <v>0.594069563592116</v>
       </c>
-      <c r="D12" s="9" t="n">
+      <c r="D12" s="10" t="n">
         <v>0.594069563592116</v>
       </c>
-      <c r="E12" s="9" t="n">
+      <c r="E12" s="10" t="n">
         <v>0.559956467059741</v>
       </c>
-      <c r="F12" s="9" t="n">
+      <c r="F12" s="10" t="n">
         <v>0.553751044629763</v>
       </c>
-      <c r="G12" s="9" t="n">
+      <c r="G12" s="10" t="n">
         <v>0.6094172934789</v>
       </c>
-      <c r="H12" s="9" t="n">
+      <c r="H12" s="10" t="n">
         <v>0.473078634496152</v>
       </c>
-      <c r="I12" s="9" t="n">
+      <c r="I12" s="10" t="n">
         <v>0.310930113498755</v>
       </c>
-      <c r="J12" s="9" t="n">
+      <c r="J12" s="10" t="n">
         <v>0.26</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="10" t="n">
         <v>0.44</v>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="M12" s="9" t="n">
+      <c r="M12" s="10" t="n">
         <v>0.37</v>
       </c>
-      <c r="N12" s="9" t="n">
+      <c r="N12" s="10" t="n">
         <v>0.47</v>
       </c>
-      <c r="O12" s="9" t="n">
+      <c r="O12" s="10" t="n">
         <v>0.358494776472968</v>
       </c>
-      <c r="P12" s="9" t="n">
+      <c r="P12" s="10" t="n">
         <v>0.34296235927199</v>
       </c>
-      <c r="Q12" s="9" t="n">
+      <c r="Q12" s="10" t="n">
         <v>0.0913159970758543</v>
       </c>
-      <c r="R12" s="9" t="n">
+      <c r="R12" s="10" t="n">
         <v>0.382351444347324</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="10" t="n">
         <v>0.7286401015179</v>
       </c>
-      <c r="D13" s="9" t="n">
+      <c r="D13" s="10" t="n">
         <v>0.7286401015179</v>
       </c>
-      <c r="E13" s="9" t="n">
+      <c r="E13" s="10" t="n">
         <v>0.661699489351116</v>
       </c>
-      <c r="F13" s="9" t="n">
+      <c r="F13" s="10" t="n">
         <v>0.650346527974745</v>
       </c>
-      <c r="G13" s="9" t="n">
+      <c r="G13" s="10" t="n">
         <v>0.687871940771877</v>
       </c>
-      <c r="H13" s="9" t="n">
+      <c r="H13" s="10" t="n">
         <v>0.582162894448399</v>
       </c>
-      <c r="I13" s="9" t="n">
+      <c r="I13" s="10" t="n">
         <v>0.353981254771086</v>
       </c>
-      <c r="J13" s="9" t="n">
+      <c r="J13" s="10" t="n">
         <v>0.33</v>
       </c>
-      <c r="K13" s="9" t="n">
+      <c r="K13" s="10" t="n">
         <v>0.56</v>
       </c>
-      <c r="L13" s="9" t="n">
+      <c r="L13" s="10" t="n">
         <v>0.42</v>
       </c>
-      <c r="M13" s="9" t="n">
+      <c r="M13" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="N13" s="9" t="n">
+      <c r="N13" s="10" t="n">
         <v>0.47</v>
       </c>
-      <c r="O13" s="9" t="n">
+      <c r="O13" s="10" t="n">
         <v>0.380555300285721</v>
       </c>
-      <c r="P13" s="9" t="n">
+      <c r="P13" s="10" t="n">
         <v>0.138343656884145</v>
       </c>
-      <c r="Q13" s="9" t="n">
+      <c r="Q13" s="10" t="n">
         <v>0.398344827590744</v>
       </c>
-      <c r="R13" s="9" t="n">
+      <c r="R13" s="10" t="n">
         <v>0.357076091526384</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="10" t="n">
         <v>0.555027179176228</v>
       </c>
-      <c r="D14" s="9" t="n">
+      <c r="D14" s="10" t="n">
         <v>0.555027179176228</v>
       </c>
-      <c r="E14" s="9" t="n">
+      <c r="E14" s="10" t="n">
         <v>0.518348570981204</v>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" s="10" t="n">
         <v>0.867444431328</v>
       </c>
-      <c r="G14" s="9" t="n">
+      <c r="G14" s="10" t="n">
         <v>0.54512400162159</v>
       </c>
-      <c r="H14" s="9" t="n">
+      <c r="H14" s="10" t="n">
         <v>0.573803477672202</v>
       </c>
-      <c r="I14" s="9" t="n">
+      <c r="I14" s="10" t="n">
         <v>0.198689640030471</v>
       </c>
-      <c r="J14" s="9" t="n">
+      <c r="J14" s="10" t="n">
         <v>0.34</v>
       </c>
-      <c r="K14" s="9" t="n">
+      <c r="K14" s="10" t="n">
         <v>0.48</v>
       </c>
-      <c r="L14" s="9" t="n">
+      <c r="L14" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="M14" s="9" t="n">
+      <c r="M14" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="N14" s="9" t="n">
+      <c r="N14" s="10" t="n">
         <v>0.46</v>
       </c>
-      <c r="O14" s="9" t="n">
+      <c r="O14" s="10" t="n">
         <v>0.437104537763042</v>
       </c>
-      <c r="P14" s="9" t="n">
+      <c r="P14" s="10" t="n">
         <v>0.257425715625404</v>
       </c>
-      <c r="Q14" s="9" t="n">
+      <c r="Q14" s="10" t="n">
         <v>0.337307357153285</v>
       </c>
-      <c r="R14" s="9" t="n">
+      <c r="R14" s="10" t="n">
         <v>0.443175749802309</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="10" t="n">
         <v>0.290858216710157</v>
       </c>
-      <c r="D15" s="9" t="n">
+      <c r="D15" s="10" t="n">
         <v>0.290858216710157</v>
       </c>
-      <c r="E15" s="9" t="n">
+      <c r="E15" s="10" t="n">
         <v>0.274029954469</v>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="10" t="n">
         <v>0.255889118413002</v>
       </c>
-      <c r="G15" s="9" t="n">
+      <c r="G15" s="10" t="n">
         <v>0.32125216826166</v>
       </c>
-      <c r="H15" s="9" t="n">
+      <c r="H15" s="10" t="n">
         <v>0.234461333980491</v>
       </c>
-      <c r="I15" s="9" t="n">
+      <c r="I15" s="10" t="n">
         <v>0.17441825098083</v>
       </c>
-      <c r="J15" s="9" t="n">
+      <c r="J15" s="10" t="n">
         <v>0.21</v>
       </c>
-      <c r="K15" s="9" t="n">
+      <c r="K15" s="10" t="n">
         <v>0.43</v>
       </c>
-      <c r="L15" s="9" t="n">
+      <c r="L15" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="M15" s="9" t="n">
+      <c r="M15" s="10" t="n">
         <v>0.37</v>
       </c>
-      <c r="N15" s="9" t="n">
+      <c r="N15" s="10" t="n">
         <v>0.49</v>
       </c>
-      <c r="O15" s="9" t="n">
+      <c r="O15" s="10" t="n">
         <v>0.341971169992378</v>
       </c>
-      <c r="P15" s="9" t="n">
+      <c r="P15" s="10" t="n">
         <v>0.846897288840176</v>
       </c>
-      <c r="Q15" s="9" t="n">
+      <c r="Q15" s="10" t="n">
         <v>0.145843912639773</v>
       </c>
-      <c r="R15" s="9" t="n">
+      <c r="R15" s="10" t="n">
         <v>0.370372201549164</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="10" t="n">
         <v>0.736603854859711</v>
       </c>
-      <c r="D16" s="9" t="n">
+      <c r="D16" s="10" t="n">
         <v>0.736603854859711</v>
       </c>
-      <c r="E16" s="9" t="n">
+      <c r="E16" s="10" t="n">
         <v>0.697732114966401</v>
       </c>
-      <c r="F16" s="9" t="n">
+      <c r="F16" s="10" t="n">
         <v>0.697732114966401</v>
       </c>
-      <c r="G16" s="9" t="n">
+      <c r="G16" s="10" t="n">
         <v>0.663619018434025</v>
       </c>
-      <c r="H16" s="9" t="n">
+      <c r="H16" s="10" t="n">
         <v>0.707218106387133</v>
       </c>
-      <c r="I16" s="9" t="n">
+      <c r="I16" s="10" t="n">
         <v>0.324728001455687</v>
       </c>
-      <c r="J16" s="9" t="n">
+      <c r="J16" s="10" t="n">
         <v>0.33</v>
       </c>
-      <c r="K16" s="9" t="n">
+      <c r="K16" s="10" t="n">
         <v>0.52</v>
       </c>
-      <c r="L16" s="9" t="n">
+      <c r="L16" s="10" t="n">
         <v>0.44</v>
       </c>
-      <c r="M16" s="9" t="n">
+      <c r="M16" s="10" t="n">
         <v>0.44</v>
       </c>
-      <c r="N16" s="9" t="n">
+      <c r="N16" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="O16" s="9" t="n">
+      <c r="O16" s="10" t="n">
         <v>0.58953760905096</v>
       </c>
-      <c r="P16" s="9" t="n">
+      <c r="P16" s="10" t="n">
         <v>0.229901871424073</v>
       </c>
-      <c r="Q16" s="9" t="n">
+      <c r="Q16" s="10" t="n">
         <v>0.236724283025347</v>
       </c>
-      <c r="R16" s="9" t="n">
+      <c r="R16" s="10" t="n">
         <v>0.549852297836994</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="10" t="n">
         <v>0.733090095728371</v>
       </c>
-      <c r="D17" s="9" t="n">
+      <c r="D17" s="10" t="n">
         <v>0.733090095728371</v>
       </c>
-      <c r="E17" s="9" t="n">
+      <c r="E17" s="10" t="n">
         <v>0.689673493568115</v>
       </c>
-      <c r="F17" s="9" t="n">
+      <c r="F17" s="10" t="n">
         <v>0.789912176738247</v>
       </c>
-      <c r="G17" s="9" t="n">
+      <c r="G17" s="10" t="n">
         <v>0.733090095728371</v>
       </c>
-      <c r="H17" s="9" t="n">
+      <c r="H17" s="10" t="n">
         <v>0.652245240166691</v>
       </c>
-      <c r="I17" s="9" t="n">
+      <c r="I17" s="10" t="n">
         <v>0.383715689446106</v>
       </c>
-      <c r="J17" s="9" t="n">
+      <c r="J17" s="10" t="n">
         <v>0.31</v>
       </c>
-      <c r="K17" s="9" t="n">
+      <c r="K17" s="10" t="n">
         <v>0.47</v>
       </c>
-      <c r="L17" s="9" t="n">
+      <c r="L17" s="10" t="n">
         <v>0.39</v>
       </c>
-      <c r="M17" s="9" t="n">
+      <c r="M17" s="10" t="n">
         <v>0.6</v>
       </c>
-      <c r="N17" s="9" t="n">
+      <c r="N17" s="10" t="n">
         <v>0.47</v>
       </c>
-      <c r="O17" s="9" t="n">
+      <c r="O17" s="10" t="n">
         <v>0.590928779614358</v>
       </c>
-      <c r="P17" s="9" t="n">
+      <c r="P17" s="10" t="n">
         <v>0.355227426694672</v>
       </c>
-      <c r="Q17" s="9" t="n">
+      <c r="Q17" s="10" t="n">
         <v>0.206933693242397</v>
       </c>
-      <c r="R17" s="9" t="n">
+      <c r="R17" s="10" t="n">
         <v>0.550860865184091</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="9" t="n">
+      <c r="C18" s="10" t="n">
         <v>0.614523406114037</v>
       </c>
-      <c r="D18" s="9" t="n">
+      <c r="D18" s="10" t="n">
         <v>0.614523406114037</v>
       </c>
-      <c r="E18" s="9" t="n">
+      <c r="E18" s="10" t="n">
         <v>0.577844797919012</v>
       </c>
-      <c r="F18" s="9" t="n">
+      <c r="F18" s="10" t="n">
         <v>0.658558041972664</v>
       </c>
-      <c r="G18" s="9" t="n">
+      <c r="G18" s="10" t="n">
         <v>0.604620228559398</v>
       </c>
-      <c r="H18" s="9" t="n">
+      <c r="H18" s="10" t="n">
         <v>0.599458740542523</v>
       </c>
-      <c r="I18" s="9" t="n">
+      <c r="I18" s="10" t="n">
         <v>0.245597279393319</v>
       </c>
-      <c r="J18" s="9" t="n">
+      <c r="J18" s="10" t="n">
         <v>0.32</v>
       </c>
-      <c r="K18" s="9" t="n">
+      <c r="K18" s="10" t="n">
         <v>0.48</v>
       </c>
-      <c r="L18" s="9" t="n">
+      <c r="L18" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="M18" s="9" t="n">
+      <c r="M18" s="10" t="n">
         <v>0.58</v>
       </c>
-      <c r="N18" s="9" t="n">
+      <c r="N18" s="10" t="n">
         <v>0.46</v>
       </c>
-      <c r="O18" s="9" t="n">
+      <c r="O18" s="10" t="n">
         <v>0.437104537763042</v>
       </c>
-      <c r="P18" s="9" t="n">
+      <c r="P18" s="10" t="n">
         <v>0.200090285864995</v>
       </c>
-      <c r="Q18" s="9" t="n">
+      <c r="Q18" s="10" t="n">
         <v>0.460711788509707</v>
       </c>
-      <c r="R18" s="9" t="n">
+      <c r="R18" s="10" t="n">
         <v>0.337413117237305</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="10" t="n">
         <v>0.695247531201919</v>
       </c>
-      <c r="D19" s="9" t="n">
+      <c r="D19" s="10" t="n">
         <v>0.695247531201919</v>
       </c>
-      <c r="E19" s="9" t="n">
+      <c r="E19" s="10" t="n">
         <v>0.643324358517786</v>
       </c>
-      <c r="F19" s="9" t="n">
+      <c r="F19" s="10" t="n">
         <v>0.67073124015801</v>
       </c>
-      <c r="G19" s="9" t="n">
+      <c r="G19" s="10" t="n">
         <v>0.68574867964066</v>
       </c>
-      <c r="H19" s="9" t="n">
+      <c r="H19" s="10" t="n">
         <v>0.548289834708421</v>
       </c>
-      <c r="I19" s="9" t="n">
+      <c r="I19" s="10" t="n">
         <v>0.364676965820379</v>
       </c>
-      <c r="J19" s="9" t="n">
+      <c r="J19" s="10" t="n">
         <v>0.3</v>
       </c>
-      <c r="K19" s="9" t="n">
+      <c r="K19" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="L19" s="9" t="n">
+      <c r="L19" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="M19" s="9" t="n">
+      <c r="M19" s="10" t="n">
         <v>0.45</v>
       </c>
-      <c r="N19" s="9" t="n">
+      <c r="N19" s="10" t="n">
         <v>0.48</v>
       </c>
-      <c r="O19" s="9" t="n">
+      <c r="O19" s="10" t="n">
         <v>0.437104537763042</v>
       </c>
-      <c r="P19" s="9" t="n">
+      <c r="P19" s="10" t="n">
         <v>0.314444647431956</v>
       </c>
-      <c r="Q19" s="9" t="n">
+      <c r="Q19" s="10" t="n">
         <v>0.445314757001293</v>
       </c>
-      <c r="R19" s="9" t="n">
+      <c r="R19" s="10" t="n">
         <v>0.300305139153555</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="10" t="n">
         <v>0.359498915240974</v>
       </c>
-      <c r="D20" s="9" t="n">
+      <c r="D20" s="10" t="n">
         <v>0.359498915240974</v>
       </c>
-      <c r="E20" s="9" t="n">
+      <c r="E20" s="10" t="n">
         <v>0.346198749609103</v>
       </c>
-      <c r="F20" s="9" t="n">
+      <c r="F20" s="10" t="n">
         <v>0.359498915240974</v>
       </c>
-      <c r="G20" s="9" t="n">
+      <c r="G20" s="10" t="n">
         <v>0.372079792662857</v>
       </c>
-      <c r="H20" s="9" t="n">
+      <c r="H20" s="10" t="n">
         <v>0.419131367502085</v>
       </c>
-      <c r="I20" s="9" t="n">
+      <c r="I20" s="10" t="n">
         <v>0.156527535286155</v>
       </c>
-      <c r="J20" s="9" t="n">
+      <c r="J20" s="10" t="n">
         <v>0.22</v>
       </c>
-      <c r="K20" s="9" t="n">
+      <c r="K20" s="10" t="n">
         <v>0.36</v>
       </c>
-      <c r="L20" s="9" t="n">
+      <c r="L20" s="10" t="n">
         <v>0.34</v>
       </c>
-      <c r="M20" s="9" t="n">
+      <c r="M20" s="10" t="n">
         <v>0.36</v>
       </c>
-      <c r="N20" s="9" t="n">
+      <c r="N20" s="10" t="n">
         <v>0.38</v>
       </c>
-      <c r="O20" s="9" t="n">
+      <c r="O20" s="10" t="n">
         <v>0.313195390181289</v>
       </c>
-      <c r="P20" s="9" t="n">
+      <c r="P20" s="10" t="n">
         <v>0.383099321658771</v>
       </c>
-      <c r="Q20" s="9" t="n">
+      <c r="Q20" s="10" t="n">
         <v>0.179421246932733</v>
       </c>
-      <c r="R20" s="9" t="n">
+      <c r="R20" s="10" t="n">
         <v>0.349510408848621</v>
       </c>
     </row>

</xml_diff>

<commit_message>
close #206: Adds support for zero-sum influencing factors
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/valores.xlsx
+++ b/input_data/data_ground_truth_01/valores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">1100049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI</t>
   </si>
   <si>
     <t xml:space="preserve">1100056</t>
@@ -458,10 +461,10 @@
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="Q22" activeCellId="0" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -678,15 +681,15 @@
         <v>0.408596234199239</v>
       </c>
       <c r="P4" s="7" t="n">
-        <v>0.244685832976119</v>
-      </c>
-      <c r="Q4" s="7" t="n">
-        <v>0.688585905681939</v>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0.729582203886894</v>
@@ -730,16 +733,16 @@
       <c r="O5" s="7" t="n">
         <v>0.486520699002306</v>
       </c>
-      <c r="P5" s="7" t="n">
-        <v>0.505871329785902</v>
+      <c r="P5" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="Q5" s="7" t="n">
-        <v>0.28745357215629</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>0.709424839994261</v>
@@ -792,7 +795,7 @@
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>0.603290170379874</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>0.659605568654101</v>
@@ -898,7 +901,7 @@
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>0.450574993784121</v>
@@ -951,7 +954,7 @@
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>0.470275035697477</v>
@@ -1004,7 +1007,7 @@
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>0.646413908506119</v>
@@ -1057,7 +1060,7 @@
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>0.594069563592116</v>
@@ -1110,7 +1113,7 @@
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>0.7286401015179</v>
@@ -1163,7 +1166,7 @@
     </row>
     <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>0.555027179176228</v>
@@ -1216,7 +1219,7 @@
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>0.290858216710157</v>
@@ -1269,7 +1272,7 @@
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>0.736603854859711</v>
@@ -1322,7 +1325,7 @@
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>0.733090095728371</v>
@@ -1375,7 +1378,7 @@
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>0.614523406114037</v>
@@ -1428,7 +1431,7 @@
     </row>
     <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>0.695247531201919</v>
@@ -1481,7 +1484,7 @@
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>0.359498915240974</v>

</xml_diff>